<commit_message>
Added ExcelReader to passTestData from Excel File Tried to implement ItestContext Tried to implement Read Data from Json File
</commit_message>
<xml_diff>
--- a/src/test/resources/Tasks.xlsx
+++ b/src/test/resources/Tasks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Narayana\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\A.NEW-DATA\SIRI\SIRIINFO--PAYROLL\WS\FrameWorkFinal\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -378,7 +378,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,6 +406,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -457,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -479,6 +485,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,7 +936,7 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="13" t="s">
         <v>92</v>
       </c>
       <c r="C11" s="1"/>
@@ -943,7 +950,7 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="13" t="s">
         <v>93</v>
       </c>
       <c r="C12" s="1"/>
@@ -955,7 +962,7 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="13" t="s">
         <v>94</v>
       </c>
       <c r="C13" s="1"/>
@@ -967,7 +974,7 @@
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="13" t="s">
         <v>97</v>
       </c>
       <c r="C14" s="1"/>
@@ -979,7 +986,7 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="13" t="s">
         <v>98</v>
       </c>
       <c r="C15" s="1"/>
@@ -991,7 +998,7 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="13" t="s">
         <v>99</v>
       </c>
       <c r="C16" s="1"/>
@@ -1003,7 +1010,7 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="13" t="s">
         <v>100</v>
       </c>
       <c r="C17" s="1"/>
@@ -1017,7 +1024,7 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="13" t="s">
         <v>102</v>
       </c>
       <c r="C18" s="1"/>
@@ -1032,7 +1039,7 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="13" t="s">
         <v>105</v>
       </c>
       <c r="C19" s="1"/>

</xml_diff>